<commit_message>
New Environment Documentation Update
Updated new environment for level, safety push before major changes to level structure.
</commit_message>
<xml_diff>
--- a/Documents/Asset List.xlsx
+++ b/Documents/Asset List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s200676\Desktop\GitRepos\ZombiePrototypeGame\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C3F347-0B71-465D-9699-0ADEBEAF8E1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA712401-7260-402C-A601-29178BF8A694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{CB8E0E31-1040-46AB-B00F-2CFC7EACC9A1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>Assets</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Player (gun)</t>
   </si>
   <si>
-    <t>0.25 x 0.25 x 0.5 Cube</t>
-  </si>
-  <si>
     <t>Arms positioned for gun</t>
   </si>
   <si>
@@ -412,6 +409,15 @@
   </si>
   <si>
     <t>512 x 512</t>
+  </si>
+  <si>
+    <t>0.5 x 0.5 x 0.5 Cube</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>City residential building, slightly taller than the platform</t>
   </si>
 </sst>
 </file>
@@ -832,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01C7D1E-BCD9-4571-8907-DC3DB6102375}">
-  <dimension ref="B1:G15"/>
+  <dimension ref="B1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,13 +864,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
@@ -882,19 +888,19 @@
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="3">
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -902,7 +908,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>19</v>
@@ -911,10 +917,10 @@
         <v>500</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -922,7 +928,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>19</v>
@@ -931,10 +937,10 @@
         <v>600</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -942,19 +948,19 @@
         <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -962,155 +968,163 @@
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="3">
         <v>6</v>
       </c>
       <c r="F7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="5">
+        <v>500</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="5">
+        <v>300</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="5">
+        <v>50</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="5">
+        <v>450</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="5">
+        <v>300</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="7">
+        <v>1000</v>
+      </c>
+      <c r="F21" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="5">
-        <v>500</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="5">
-        <v>300</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="5">
-        <v>50</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="5">
-        <v>450</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="5">
-        <v>300</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="7">
-        <v>1000</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>43</v>
+      <c r="G21" s="7" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Environment GreyBox/Asset List Update
Greyboxed environment is now in Level.
</commit_message>
<xml_diff>
--- a/Documents/Asset List.xlsx
+++ b/Documents/Asset List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s200676\Desktop\GitRepos\ZombiePrototypeGame\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA712401-7260-402C-A601-29178BF8A694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70D45E4-F021-450A-BFB8-AF6B05D28D5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{CB8E0E31-1040-46AB-B00F-2CFC7EACC9A1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="71">
   <si>
     <t>Assets</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Ramp</t>
   </si>
   <si>
-    <t>Ramp Platform</t>
-  </si>
-  <si>
     <t>Zombie (body)</t>
   </si>
   <si>
@@ -231,22 +228,6 @@
   </si>
   <si>
     <r>
-      <t>Platform which seamlessly</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> attaches to ramps</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Body size </t>
     </r>
     <r>
@@ -381,18 +362,12 @@
     <t>1 x 2 x 3 Cube</t>
   </si>
   <si>
-    <t>1 x 0.25 x 2 Cube</t>
-  </si>
-  <si>
     <t>1024 x 1024</t>
   </si>
   <si>
     <t>2048 x 2048</t>
   </si>
   <si>
-    <t>512 x  512</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -414,10 +389,245 @@
     <t>0.5 x 0.5 x 0.5 Cube</t>
   </si>
   <si>
-    <t>Building</t>
-  </si>
-  <si>
-    <t>City residential building, slightly taller than the platform</t>
+    <t>Building 1</t>
+  </si>
+  <si>
+    <t>Building 2</t>
+  </si>
+  <si>
+    <t>25 x 50 x 25 Cube</t>
+  </si>
+  <si>
+    <t>25 x 70 x 25 Cube</t>
+  </si>
+  <si>
+    <t>Block of Land</t>
+  </si>
+  <si>
+    <t>Construction Site</t>
+  </si>
+  <si>
+    <t>Fence</t>
+  </si>
+  <si>
+    <t>25 x 1 x 25 Cube</t>
+  </si>
+  <si>
+    <t>0.5 x 2.5 x 4 Cube</t>
+  </si>
+  <si>
+    <t>Scaffold Beams</t>
+  </si>
+  <si>
+    <t>1.5 x 5 x 1.5 Cube</t>
+  </si>
+  <si>
+    <t>Dump Truck</t>
+  </si>
+  <si>
+    <t>4 x 5 x 15</t>
+  </si>
+  <si>
+    <t>Support Beam</t>
+  </si>
+  <si>
+    <t>12 x 1 x 1 Cube</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">City residential building, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>slightly taller</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> than the platform</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">City residential building, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>taller than</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the platform</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Space below the player with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lights and construction Assets</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>measurement of the ground</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the environment is placed on</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Placeholder walls </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>placed around the Construction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Site</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>placeholder beam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> which will stack on top of each other</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A beam which can be stacked into</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> a pile on the ground</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A large construction </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dump truck with dirt in the back</t>
+    </r>
+  </si>
+  <si>
+    <t>Spotlights</t>
+  </si>
+  <si>
+    <t>Spotlights littered around the construction site</t>
+  </si>
+  <si>
+    <t>0.5 x 7.5 x 0.5 Cube</t>
+  </si>
+  <si>
+    <t>Crane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parallel to platform, arm stretched with lights </t>
+  </si>
+  <si>
+    <t>35 x 47.5 x 3</t>
   </si>
 </sst>
 </file>
@@ -503,7 +713,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -522,6 +732,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -838,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01C7D1E-BCD9-4571-8907-DC3DB6102375}">
-  <dimension ref="B1:G21"/>
+  <dimension ref="B1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,13 +1080,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
@@ -888,19 +1104,19 @@
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E3" s="3">
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -908,39 +1124,39 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="3">
         <v>500</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="3">
         <v>600</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -948,183 +1164,339 @@
         <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E7" s="3">
         <v>6</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="3">
+        <v>6</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="3">
+        <v>6</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="C10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="3">
+        <v>6</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="3">
+        <v>12</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="3">
+        <v>120</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="3">
+        <v>6</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="3">
+        <v>250</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="3">
+        <v>30</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="3">
+        <v>300</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="5">
-        <v>500</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="5">
-        <v>300</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="5">
-        <v>50</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" s="5"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="14"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="E18" s="5">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E19" s="5">
         <v>300</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="5">
+        <v>50</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="5">
+        <v>450</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="5">
+        <v>300</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="7">
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="15"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="7">
         <v>1000</v>
       </c>
-      <c r="F21" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>42</v>
+      <c r="F24" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Skybox and LDD
Replaced Corilas with Stormy night, added features into LDD.
</commit_message>
<xml_diff>
--- a/Documents/Asset List.xlsx
+++ b/Documents/Asset List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s200676\Desktop\GitRepos\ZombiePrototypeGame\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70D45E4-F021-450A-BFB8-AF6B05D28D5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A15C684-BC67-4F53-B1A4-6275156B113F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{CB8E0E31-1040-46AB-B00F-2CFC7EACC9A1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{CB8E0E31-1040-46AB-B00F-2CFC7EACC9A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
   <si>
     <t>Assets</t>
   </si>
@@ -428,9 +428,6 @@
     <t>4 x 5 x 15</t>
   </si>
   <si>
-    <t>Support Beam</t>
-  </si>
-  <si>
     <t>12 x 1 x 1 Cube</t>
   </si>
   <si>
@@ -628,6 +625,9 @@
   </si>
   <si>
     <t>35 x 47.5 x 3</t>
+  </si>
+  <si>
+    <t>Wooden Plank</t>
   </si>
 </sst>
 </file>
@@ -1057,7 +1057,7 @@
   <dimension ref="B1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,7 +1184,7 @@
         <v>42</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>44</v>
@@ -1195,14 +1195,16 @@
       <c r="F7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>45</v>
@@ -1213,14 +1215,16 @@
       <c r="F8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="4"/>
+      <c r="G8" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>49</v>
@@ -1238,7 +1242,7 @@
         <v>46</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>49</v>
@@ -1256,7 +1260,7 @@
         <v>48</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>50</v>
@@ -1274,7 +1278,7 @@
         <v>51</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>52</v>
@@ -1289,13 +1293,13 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="E13" s="3">
         <v>6</v>
@@ -1310,7 +1314,7 @@
         <v>53</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>54</v>
@@ -1325,13 +1329,13 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="E15" s="3">
         <v>30</v>
@@ -1343,13 +1347,13 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="E16" s="3">
         <v>300</v>
@@ -1357,7 +1361,9 @@
       <c r="F16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">

</xml_diff>

<commit_message>
Final Push of Complete Assignment, before zipping
</commit_message>
<xml_diff>
--- a/Documents/Asset List.xlsx
+++ b/Documents/Asset List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s200676\Desktop\GitRepos\ZombiePrototypeGame\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A15C684-BC67-4F53-B1A4-6275156B113F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94B376E-D7F2-427B-9734-C8A52B3CDEFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{CB8E0E31-1040-46AB-B00F-2CFC7EACC9A1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
   <si>
     <t>Assets</t>
   </si>
@@ -401,33 +401,12 @@
     <t>25 x 70 x 25 Cube</t>
   </si>
   <si>
-    <t>Block of Land</t>
-  </si>
-  <si>
-    <t>Construction Site</t>
-  </si>
-  <si>
-    <t>Fence</t>
-  </si>
-  <si>
-    <t>25 x 1 x 25 Cube</t>
-  </si>
-  <si>
-    <t>0.5 x 2.5 x 4 Cube</t>
-  </si>
-  <si>
     <t>Scaffold Beams</t>
   </si>
   <si>
     <t>1.5 x 5 x 1.5 Cube</t>
   </si>
   <si>
-    <t>Dump Truck</t>
-  </si>
-  <si>
-    <t>4 x 5 x 15</t>
-  </si>
-  <si>
     <t>12 x 1 x 1 Cube</t>
   </si>
   <si>
@@ -484,22 +463,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Space below the player with </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>lights and construction Assets</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">A </t>
     </r>
     <r>
@@ -511,58 +474,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>measurement of the ground</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the environment is placed on</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Placeholder walls </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>placed around the Construction</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Site</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>placeholder beam</t>
     </r>
     <r>
@@ -593,31 +504,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">A large construction </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dump truck with dirt in the back</t>
-    </r>
-  </si>
-  <si>
-    <t>Spotlights</t>
-  </si>
-  <si>
-    <t>Spotlights littered around the construction site</t>
-  </si>
-  <si>
-    <t>0.5 x 7.5 x 0.5 Cube</t>
-  </si>
-  <si>
     <t>Crane</t>
   </si>
   <si>
@@ -627,7 +513,7 @@
     <t>35 x 47.5 x 3</t>
   </si>
   <si>
-    <t>Wooden Plank</t>
+    <t>Metal Beam</t>
   </si>
 </sst>
 </file>
@@ -1054,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01C7D1E-BCD9-4571-8907-DC3DB6102375}">
-  <dimension ref="B1:G24"/>
+  <dimension ref="B1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I13" sqref="H13:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,7 +1070,7 @@
         <v>42</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>44</v>
@@ -1204,7 +1090,7 @@
         <v>43</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>45</v>
@@ -1221,287 +1107,201 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="E9" s="3">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="3">
         <v>6</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="3">
+        <v>300</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="5">
+        <v>500</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="5">
+        <v>300</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="5">
         <v>50</v>
       </c>
-      <c r="E11" s="3">
-        <v>12</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="F15" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="5">
+        <v>450</v>
+      </c>
+      <c r="F16" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="3">
-        <v>120</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="3">
-        <v>6</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="3">
-        <v>250</v>
-      </c>
-      <c r="F14" s="4" t="s">
+      <c r="G16" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="5">
+        <v>300</v>
+      </c>
+      <c r="F17" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="3">
-        <v>30</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="3">
-        <v>300</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="14"/>
+      <c r="G17" s="12" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="5">
-        <v>500</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="B18" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="15"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="5">
-        <v>300</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="5">
-        <v>50</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="5">
-        <v>450</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="5">
-        <v>300</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="15"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
+      <c r="B19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C19" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E19" s="7">
         <v>1000</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F19" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G19" s="13" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>